<commit_message>
compelte instruction in every stage and get all control signal(maybe)...
</commit_message>
<xml_diff>
--- a/doc/pr2_design/instruction.xlsx
+++ b/doc/pr2_design/instruction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="3030" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="189">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -294,10 +294,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SP←R[x]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>10001XXXIIIIIIII</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -330,202 +326,471 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>R[x]←SP+sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LI rx immediate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[x]←zero_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[y]←R[x]+sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LW rx ry immediate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW rx ry immediate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEM[R[x]+sign_extend(immediate)]←R[y]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW_SP rx immediate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEM[SP+sign_extend(immediate)]←R[x]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10000XXXIIIIIIII</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10010XXXIIIIIIII</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10100XXXIIIIIIII</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10101XXXYYY0IIII</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10110XXXYYYIIIII</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10111XXXYYYIIIII</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>BTEQZ</t>
+  </si>
+  <si>
+    <t>11001IIIIIIII000</t>
+  </si>
+  <si>
+    <t>BEQZ</t>
+  </si>
+  <si>
+    <t>11010XXXIIIIIIII</t>
+  </si>
+  <si>
+    <t>BNEZ</t>
+  </si>
+  <si>
+    <t>11011XXXIIIIIIII</t>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11000IIIIIIIIIII</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B immediate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[y]←MEM[R[x]+sign_extend(immediate)]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BEQZ rx immediate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (R[x]=0) then PC←PC+sign)extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BTEQZ immediate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (T=0) then PC←PC+sign)extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BNEZ rx immediate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (R[x]!=0) then PC←PC+sign)extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*JRRA</t>
+  </si>
+  <si>
+    <t>JR</t>
+  </si>
+  <si>
+    <t>J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11101XXX00000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1110000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC←PC+sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JRRA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC←RA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JR rx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC←R[x]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC←PC+4</t>
+  </si>
+  <si>
+    <t>PC←PC+4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←IH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rx←A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←PC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←rx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IH←A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP←rx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←rx, B←ry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C←rx&amp;ry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rx←C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C←rx|ry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>←</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>ry</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>←</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+      </rPr>
+      <t>~A</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rx←B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←ry, B←sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rx←C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C←A&lt;&lt;B(B=0时A&lt;&lt;8)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C←A&gt;&gt;B(算术右移，B=0时A&gt;&gt;8)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←rx, B←ry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rz←C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP←SP+sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←ry, B←sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←SP, B←sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C←A+B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C←A-B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP←C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D←MEM[C]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rx←D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←SP, B←sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←rx, B←sign_extend(immediate), C←SP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D←B+C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEM[D]←A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←rx, B←sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C←A+B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rx←C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (A&lt;B) T←1 else T←0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rx←C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←zero_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>ADDSP3 rx immediate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>R[x]←SP+sign_extend(immediate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LI rx immediate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R[x]←zero_extend(immediate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ADDIU3 rx immediate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R[y]←R[x]+sign_extend(immediate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LW rx ry immediate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SW rx ry immediate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MEM[R[x]+sign_extend(immediate)]←R[y]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SW_SP rx immediate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MEM[SP+sign_extend(immediate)]←R[x]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10000XXXIIIIIIII</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10010XXXIIIIIIII</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10100XXXIIIIIIII</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10101XXXYYY0IIII</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10110XXXYYYIIIII</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10111XXXYYYIIIII</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>BTEQZ</t>
-  </si>
-  <si>
-    <t>11001IIIIIIII000</t>
-  </si>
-  <si>
-    <t>BEQZ</t>
-  </si>
-  <si>
-    <t>11010XXXIIIIIIII</t>
-  </si>
-  <si>
-    <t>BNEZ</t>
-  </si>
-  <si>
-    <t>11011XXXIIIIIIII</t>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11000IIIIIIIIIII</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B immediate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R[y]←MEM[R[x]+sign_extend(immediate)]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BEQZ rx immediate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if (R[x]=0) then PC←PC+sign)extend(immediate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BTEQZ immediate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if (T=0) then PC←PC+sign)extend(immediate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BNEZ rx immediate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if (R[x]!=0) then PC←PC+sign)extend(immediate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*JRRA</t>
-  </si>
-  <si>
-    <t>JR</t>
-  </si>
-  <si>
-    <t>J</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11101XXX00000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1110000000000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC←PC+sign_extend(immediate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JRRA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC←RA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JR rx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC←R[x]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NOP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NOP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NOP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MEM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WB</t>
+    <t>ADDIU3 rx ry immediate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C←A+B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ry←C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←rx, B←sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←rx, B←sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D←MEM[C]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ry←D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D←A+B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEM[D]←C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←rx, B←sign_extend(immediate), C←ry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←sign_extend(immediate), B←A&lt;&lt;2, C←PC+B, PC←C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (A!=B)T=1 else T=0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (A&lt;B)T=1 else T=0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC←PC+4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(T=0) A←sign_extend(immediate), B←A&lt;&lt;2, C←PC+B, PC←C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←rx, if (A=0) B←sign_extend(immediate), C←B&lt;&lt;2,D←PC+C,PC←D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←rx, if (A!=0) B←sign_extend(immediate), C←B&lt;&lt;2,D←PC+C,PC←D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←RA, PC←RA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←rx, PC←A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -893,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -902,6 +1167,10 @@
     <col min="3" max="3" width="21.75" customWidth="1"/>
     <col min="4" max="4" width="21.375" customWidth="1"/>
     <col min="5" max="5" width="25.875" customWidth="1"/>
+    <col min="6" max="6" width="9.375" customWidth="1"/>
+    <col min="7" max="7" width="39.25" customWidth="1"/>
+    <col min="8" max="8" width="24.25" customWidth="1"/>
+    <col min="9" max="9" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.15">
@@ -921,19 +1190,19 @@
         <v>32</v>
       </c>
       <c r="F1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" t="s">
         <v>128</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>129</v>
-      </c>
-      <c r="H1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I1" t="s">
-        <v>131</v>
-      </c>
-      <c r="J1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
@@ -952,6 +1221,15 @@
       <c r="E2" t="s">
         <v>33</v>
       </c>
+      <c r="F2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
@@ -969,6 +1247,15 @@
       <c r="E3" t="s">
         <v>36</v>
       </c>
+      <c r="F3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J3" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
@@ -986,6 +1273,15 @@
       <c r="E4" t="s">
         <v>37</v>
       </c>
+      <c r="F4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
@@ -1003,6 +1299,15 @@
       <c r="E5" t="s">
         <v>39</v>
       </c>
+      <c r="F5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J5" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -1020,6 +1325,18 @@
       <c r="E6" t="s">
         <v>41</v>
       </c>
+      <c r="F6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G6" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" t="s">
+        <v>139</v>
+      </c>
+      <c r="J6" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
@@ -1037,6 +1354,18 @@
       <c r="E7" t="s">
         <v>43</v>
       </c>
+      <c r="F7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
@@ -1054,6 +1383,18 @@
       <c r="E8" t="s">
         <v>46</v>
       </c>
+      <c r="F8" t="s">
+        <v>130</v>
+      </c>
+      <c r="G8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H8" t="s">
+        <v>143</v>
+      </c>
+      <c r="J8" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
@@ -1071,6 +1412,15 @@
       <c r="E9" t="s">
         <v>47</v>
       </c>
+      <c r="F9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" t="s">
+        <v>138</v>
+      </c>
+      <c r="H9" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
@@ -1088,6 +1438,15 @@
       <c r="E10" t="s">
         <v>50</v>
       </c>
+      <c r="F10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" t="s">
+        <v>138</v>
+      </c>
+      <c r="H10" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
@@ -1105,6 +1464,18 @@
       <c r="E11" t="s">
         <v>52</v>
       </c>
+      <c r="F11" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" t="s">
+        <v>152</v>
+      </c>
+      <c r="H11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -1122,6 +1493,18 @@
       <c r="E12" t="s">
         <v>53</v>
       </c>
+      <c r="F12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" t="s">
+        <v>148</v>
+      </c>
+      <c r="J12" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
@@ -1139,6 +1522,18 @@
       <c r="E13" t="s">
         <v>55</v>
       </c>
+      <c r="F13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G13" t="s">
+        <v>149</v>
+      </c>
+      <c r="H13" t="s">
+        <v>154</v>
+      </c>
+      <c r="J13" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
@@ -1156,6 +1551,18 @@
       <c r="E14" t="s">
         <v>57</v>
       </c>
+      <c r="F14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" t="s">
+        <v>138</v>
+      </c>
+      <c r="H14" t="s">
+        <v>155</v>
+      </c>
+      <c r="J14" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
@@ -1171,7 +1578,19 @@
         <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>151</v>
+      </c>
+      <c r="F15" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H15" t="s">
+        <v>154</v>
+      </c>
+      <c r="J15" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
@@ -1182,16 +1601,31 @@
         <v>70</v>
       </c>
       <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
         <v>74</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>75</v>
       </c>
-      <c r="E16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F16" t="s">
+        <v>130</v>
+      </c>
+      <c r="G16" t="s">
+        <v>159</v>
+      </c>
+      <c r="H16" t="s">
+        <v>154</v>
+      </c>
+      <c r="I16" t="s">
+        <v>157</v>
+      </c>
+      <c r="J16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1199,16 +1633,28 @@
         <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+        <v>88</v>
+      </c>
+      <c r="F17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" t="s">
+        <v>161</v>
+      </c>
+      <c r="I17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -1216,16 +1662,28 @@
         <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
         <v>77</v>
       </c>
-      <c r="E18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G18" t="s">
+        <v>163</v>
+      </c>
+      <c r="H18" t="s">
+        <v>164</v>
+      </c>
+      <c r="J18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -1233,16 +1691,25 @@
         <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" t="s">
         <v>79</v>
       </c>
-      <c r="E19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F19" t="s">
+        <v>130</v>
+      </c>
+      <c r="G19" t="s">
+        <v>163</v>
+      </c>
+      <c r="H19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -1253,13 +1720,25 @@
         <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+        <v>80</v>
+      </c>
+      <c r="F20" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" t="s">
+        <v>153</v>
+      </c>
+      <c r="H20" t="s">
+        <v>154</v>
+      </c>
+      <c r="J20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -1267,16 +1746,25 @@
         <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+        <v>82</v>
+      </c>
+      <c r="F21" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" t="s">
+        <v>168</v>
+      </c>
+      <c r="J21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -1284,16 +1772,28 @@
         <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+        <v>83</v>
+      </c>
+      <c r="F22" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" t="s">
+        <v>173</v>
+      </c>
+      <c r="H22" t="s">
+        <v>171</v>
+      </c>
+      <c r="J22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -1301,16 +1801,31 @@
         <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+        <v>105</v>
+      </c>
+      <c r="F23" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" t="s">
+        <v>171</v>
+      </c>
+      <c r="I23" t="s">
+        <v>175</v>
+      </c>
+      <c r="J23" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -1318,129 +1833,180 @@
         <v>70</v>
       </c>
       <c r="C24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" t="s">
+        <v>179</v>
+      </c>
+      <c r="H24" t="s">
+        <v>177</v>
+      </c>
+      <c r="I24" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" t="s">
+        <v>130</v>
+      </c>
+      <c r="G25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
         <v>97</v>
       </c>
-      <c r="D24" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
+      <c r="D26" t="s">
+        <v>108</v>
+      </c>
+      <c r="E26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" t="s">
+        <v>130</v>
+      </c>
+      <c r="G26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
         <v>98</v>
       </c>
-      <c r="B25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" t="s">
         <v>106</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E27" t="s">
         <v>107</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F27" t="s">
+        <v>130</v>
+      </c>
+      <c r="G27" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" t="s">
+        <v>111</v>
+      </c>
+      <c r="F28" t="s">
+        <v>130</v>
+      </c>
+      <c r="G28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" t="s">
+        <v>119</v>
+      </c>
+      <c r="F29" t="s">
+        <v>130</v>
+      </c>
+      <c r="G29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
-        <v>101</v>
-      </c>
-      <c r="B27" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" t="s">
-        <v>109</v>
-      </c>
-      <c r="E27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
-        <v>103</v>
-      </c>
-      <c r="B28" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" t="s">
-        <v>113</v>
-      </c>
-      <c r="E28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
-        <v>115</v>
-      </c>
-      <c r="B29" t="s">
-        <v>117</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="E30" t="s">
         <v>121</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F30" t="s">
+        <v>130</v>
+      </c>
+      <c r="G30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>116</v>
-      </c>
-      <c r="B30" t="s">
-        <v>117</v>
-      </c>
-      <c r="C30" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="B31" t="s">
         <v>123</v>
-      </c>
-      <c r="E30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" t="s">
-        <v>126</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>127</v>
+        <v>124</v>
+      </c>
+      <c r="F31" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a signal, update instruction, finish ModuleInterface
</commit_message>
<xml_diff>
--- a/doc/pr2_design/instruction.xlsx
+++ b/doc/pr2_design/instruction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="4890" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="215">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -865,6 +865,33 @@
   </si>
   <si>
     <t>110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALUsrc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1231,10 +1258,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1248,7 +1278,7 @@
     <col min="9" max="9" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1285,23 +1315,26 @@
       <c r="L1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="N1" t="s">
         <v>194</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>190</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>193</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>192</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1332,8 +1365,8 @@
       <c r="L2" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="M2">
-        <v>0</v>
+      <c r="M2" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1347,8 +1380,11 @@
       <c r="Q2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1379,8 +1415,8 @@
       <c r="L3" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="M3">
-        <v>0</v>
+      <c r="M3" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -1394,8 +1430,11 @@
       <c r="Q3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1426,8 +1465,8 @@
       <c r="L4" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M4">
-        <v>0</v>
+      <c r="M4" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1441,8 +1480,11 @@
       <c r="Q4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1473,8 +1515,8 @@
       <c r="L5" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M5">
-        <v>0</v>
+      <c r="M5" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1488,8 +1530,11 @@
       <c r="Q5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1523,8 +1568,8 @@
       <c r="L6" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="M6">
-        <v>0</v>
+      <c r="M6" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1538,8 +1583,11 @@
       <c r="Q6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1573,8 +1621,8 @@
       <c r="L7" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="M7">
-        <v>0</v>
+      <c r="M7" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -1588,8 +1636,11 @@
       <c r="Q7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1623,8 +1674,8 @@
       <c r="L8" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="M8">
-        <v>0</v>
+      <c r="M8" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -1638,8 +1689,11 @@
       <c r="Q8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1670,23 +1724,26 @@
       <c r="L9" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="M9">
-        <v>0</v>
+      <c r="M9" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
         <v>1</v>
       </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1717,14 +1774,14 @@
       <c r="L10" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="M10">
-        <v>1</v>
+      <c r="M10" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N10">
         <v>1</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1732,8 +1789,11 @@
       <c r="Q10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1767,8 +1827,8 @@
       <c r="L11" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="M11">
-        <v>0</v>
+      <c r="M11" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -1782,8 +1842,11 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1817,8 +1880,8 @@
       <c r="L12" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="M12">
-        <v>0</v>
+      <c r="M12" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1832,8 +1895,11 @@
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1867,8 +1933,8 @@
       <c r="L13" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="M13">
-        <v>0</v>
+      <c r="M13" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -1882,8 +1948,11 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1917,8 +1986,8 @@
       <c r="L14" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="M14">
-        <v>0</v>
+      <c r="M14" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -1932,8 +2001,11 @@
       <c r="Q14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -1967,8 +2039,8 @@
       <c r="L15" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M15">
-        <v>0</v>
+      <c r="M15" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -1982,8 +2054,11 @@
       <c r="Q15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -2020,23 +2095,26 @@
       <c r="L16" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M16">
-        <v>0</v>
+      <c r="M16" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="N16">
         <v>0</v>
       </c>
       <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
         <v>1</v>
       </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
       <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -2070,8 +2148,8 @@
       <c r="L17" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M17">
-        <v>0</v>
+      <c r="M17" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -2080,13 +2158,16 @@
         <v>0</v>
       </c>
       <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
         <v>1</v>
       </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -2120,8 +2201,8 @@
       <c r="L18" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M18">
-        <v>0</v>
+      <c r="M18" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="N18">
         <v>0</v>
@@ -2135,8 +2216,11 @@
       <c r="Q18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -2167,23 +2251,26 @@
       <c r="L19" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="M19">
-        <v>0</v>
+      <c r="M19" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
         <v>1</v>
       </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
       <c r="P19">
         <v>0</v>
       </c>
       <c r="Q19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -2217,8 +2304,8 @@
       <c r="L20" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M20">
-        <v>0</v>
+      <c r="M20" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -2232,8 +2319,11 @@
       <c r="Q20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -2264,8 +2354,8 @@
       <c r="L21" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M21">
-        <v>0</v>
+      <c r="M21" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N21">
         <v>0</v>
@@ -2279,8 +2369,11 @@
       <c r="Q21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -2314,8 +2407,8 @@
       <c r="L22" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M22">
-        <v>0</v>
+      <c r="M22" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -2329,8 +2422,11 @@
       <c r="Q22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -2367,23 +2463,26 @@
       <c r="L23" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M23">
-        <v>0</v>
+      <c r="M23" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="N23">
         <v>0</v>
       </c>
       <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
         <v>1</v>
       </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
       <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -2417,8 +2516,8 @@
       <c r="L24" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M24">
-        <v>0</v>
+      <c r="M24" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -2427,13 +2526,16 @@
         <v>0</v>
       </c>
       <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
         <v>1</v>
       </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -2461,8 +2563,8 @@
       <c r="L25" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M25">
-        <v>0</v>
+      <c r="M25" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -2476,8 +2578,11 @@
       <c r="Q25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -2505,8 +2610,8 @@
       <c r="L26" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M26">
-        <v>0</v>
+      <c r="M26" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -2520,8 +2625,11 @@
       <c r="Q26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -2549,8 +2657,8 @@
       <c r="L27" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M27">
-        <v>0</v>
+      <c r="M27" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -2564,8 +2672,11 @@
       <c r="Q27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -2593,8 +2704,8 @@
       <c r="L28" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M28">
-        <v>0</v>
+      <c r="M28" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -2608,8 +2719,11 @@
       <c r="Q28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -2637,8 +2751,8 @@
       <c r="L29" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M29">
-        <v>0</v>
+      <c r="M29" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -2652,8 +2766,11 @@
       <c r="Q29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>113</v>
       </c>
@@ -2681,8 +2798,8 @@
       <c r="L30" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M30">
-        <v>0</v>
+      <c r="M30" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N30">
         <v>0</v>
@@ -2696,8 +2813,11 @@
       <c r="Q30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="R30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -2719,8 +2839,8 @@
       <c r="L31" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="M31">
-        <v>0</v>
+      <c r="M31" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="N31">
         <v>0</v>
@@ -2732,6 +2852,9 @@
         <v>0</v>
       </c>
       <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
complete Branch in struction.xlsx
</commit_message>
<xml_diff>
--- a/doc/pr2_design/instruction.xlsx
+++ b/doc/pr2_design/instruction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="5820" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="218">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -892,6 +892,18 @@
   </si>
   <si>
     <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1261,10 +1273,10 @@
   <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2558,7 +2570,7 @@
         <v>180</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>198</v>
@@ -2605,7 +2617,7 @@
         <v>184</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>198</v>
@@ -2652,7 +2664,7 @@
         <v>185</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>198</v>
@@ -2699,7 +2711,7 @@
         <v>186</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>198</v>
@@ -2746,7 +2758,7 @@
         <v>187</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>198</v>
@@ -2793,7 +2805,7 @@
         <v>188</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>198</v>

</xml_diff>

<commit_message>
fixed datapath and finish linking in ID
</commit_message>
<xml_diff>
--- a/doc/pr2_design/instruction.xlsx
+++ b/doc/pr2_design/instruction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="6750" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="219">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -904,6 +904,10 @@
   </si>
   <si>
     <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegWrite</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1270,13 +1274,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I31" sqref="I31"/>
+      <selection pane="bottomRight" activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1290,7 +1294,7 @@
     <col min="9" max="9" width="10.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1345,8 +1349,11 @@
       <c r="R1" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1395,8 +1402,11 @@
       <c r="R2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1445,8 +1455,11 @@
       <c r="R3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1495,8 +1508,11 @@
       <c r="R4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1545,8 +1561,11 @@
       <c r="R5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1598,8 +1617,11 @@
       <c r="R6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1651,8 +1673,11 @@
       <c r="R7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1704,8 +1729,11 @@
       <c r="R8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1754,8 +1782,11 @@
       <c r="R9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1804,8 +1835,11 @@
       <c r="R10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1857,8 +1891,11 @@
       <c r="R11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1910,8 +1947,11 @@
       <c r="R12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1963,8 +2003,11 @@
       <c r="R13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2016,8 +2059,11 @@
       <c r="R14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -2069,8 +2115,11 @@
       <c r="R15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -2125,8 +2174,11 @@
       <c r="R16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -2178,8 +2230,11 @@
       <c r="R17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -2231,8 +2286,11 @@
       <c r="R18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -2281,8 +2339,11 @@
       <c r="R19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -2334,8 +2395,11 @@
       <c r="R20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -2384,8 +2448,11 @@
       <c r="R21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -2437,8 +2504,11 @@
       <c r="R22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -2493,8 +2563,11 @@
       <c r="R23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -2546,8 +2619,11 @@
       <c r="R24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -2593,8 +2669,11 @@
       <c r="R25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>96</v>
       </c>
@@ -2640,8 +2719,11 @@
       <c r="R26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>98</v>
       </c>
@@ -2687,8 +2769,11 @@
       <c r="R27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -2734,8 +2819,11 @@
       <c r="R28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -2781,8 +2869,11 @@
       <c r="R29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>113</v>
       </c>
@@ -2828,8 +2919,11 @@
       <c r="R30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="S30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>122</v>
       </c>
@@ -2867,6 +2961,9 @@
         <v>0</v>
       </c>
       <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finish ID_EX and Treg
</commit_message>
<xml_diff>
--- a/doc/pr2_design/instruction.xlsx
+++ b/doc/pr2_design/instruction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8610" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="9540" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="228">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -900,23 +900,50 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>NOT*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLT*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLTI*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0000000000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>JRRA*</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>NOT*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLT*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SLTI*</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000000000000000</t>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rx←A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ry+sign_extend(immediate)]←RA</t>
+  </si>
+  <si>
+    <t>BPC←PCA</t>
+  </si>
+  <si>
+    <t>BTEQZPC←PCi</t>
+  </si>
+  <si>
+    <t>rx=0) then PC←PCA</t>
+  </si>
+  <si>
+    <t>rx!=0) then PC←PCA</t>
+  </si>
+  <si>
+    <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1286,17 +1313,17 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="21.75" customWidth="1"/>
     <col min="4" max="4" width="21.375" customWidth="1"/>
-    <col min="5" max="5" width="25.875" customWidth="1"/>
+    <col min="5" max="5" width="75" customWidth="1"/>
     <col min="6" max="6" width="9.375" customWidth="1"/>
     <col min="7" max="7" width="39.25" customWidth="1"/>
     <col min="8" max="8" width="24.25" customWidth="1"/>
@@ -1370,7 +1397,7 @@
         <v>118</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D2" t="s">
         <v>119</v>
@@ -1732,7 +1759,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -1788,7 +1815,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
@@ -2345,7 +2372,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B20" t="s">
         <v>66</v>
@@ -2475,7 +2502,7 @@
         <v>163</v>
       </c>
       <c r="J22" t="s">
-        <v>135</v>
+        <v>221</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>191</v>
@@ -2484,7 +2511,7 @@
         <v>193</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>204</v>
+        <v>227</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -2878,7 +2905,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B30" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
fixed the bug of zero extend in sll,sra
</commit_message>
<xml_diff>
--- a/doc/pr2_design/instruction.xlsx
+++ b/doc/pr2_design/instruction.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$31</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="223">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -603,10 +606,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A←ry, B←sign_extend(immediate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>rx←C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -631,10 +630,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A←ry, B←sign_extend(immediate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>A←SP, B←sign_extend(immediate)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -920,30 +915,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>rx←A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>rx←A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ry+sign_extend(immediate)]←RA</t>
-  </si>
-  <si>
-    <t>BPC←PCA</t>
-  </si>
-  <si>
-    <t>BTEQZPC←PCi</t>
-  </si>
-  <si>
-    <t>rx=0) then PC←PCA</t>
-  </si>
-  <si>
-    <t>rx!=0) then PC←PCA</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←ry, B←zero_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A←ry, B←zero_extend(immediate)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1312,11 +1300,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M22" sqref="M22"/>
+      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1362,31 +1350,31 @@
         <v>124</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="N1" t="s">
+        <v>187</v>
+      </c>
+      <c r="O1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P1" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>185</v>
+      </c>
+      <c r="R1" t="s">
         <v>184</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="N1" t="s">
-        <v>189</v>
-      </c>
-      <c r="O1" t="s">
-        <v>185</v>
-      </c>
-      <c r="P1" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>187</v>
-      </c>
-      <c r="R1" t="s">
-        <v>186</v>
-      </c>
       <c r="S1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
@@ -1397,7 +1385,7 @@
         <v>118</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D2" t="s">
         <v>119</v>
@@ -1406,13 +1394,13 @@
         <v>125</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M2" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1450,7 +1438,7 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G3" t="s">
         <v>127</v>
@@ -1459,13 +1447,13 @@
         <v>128</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="M3" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -1512,13 +1500,13 @@
         <v>128</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1565,13 +1553,13 @@
         <v>131</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M5" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1618,13 +1606,13 @@
         <v>132</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M6" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1642,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.15">
@@ -1674,13 +1662,13 @@
         <v>135</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -1730,13 +1718,13 @@
         <v>135</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -1759,7 +1747,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -1786,13 +1774,13 @@
         <v>139</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1815,7 +1803,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
@@ -1836,16 +1824,16 @@
         <v>133</v>
       </c>
       <c r="H10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1889,16 +1877,16 @@
         <v>133</v>
       </c>
       <c r="H11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -1939,22 +1927,22 @@
         <v>125</v>
       </c>
       <c r="G12" t="s">
-        <v>147</v>
+        <v>221</v>
       </c>
       <c r="H12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1995,22 +1983,22 @@
         <v>125</v>
       </c>
       <c r="G13" t="s">
+        <v>222</v>
+      </c>
+      <c r="H13" t="s">
+        <v>142</v>
+      </c>
+      <c r="J13" t="s">
         <v>140</v>
       </c>
-      <c r="H13" t="s">
-        <v>143</v>
-      </c>
-      <c r="J13" t="s">
-        <v>141</v>
-      </c>
       <c r="K13" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -2051,22 +2039,22 @@
         <v>125</v>
       </c>
       <c r="G14" t="s">
+        <v>143</v>
+      </c>
+      <c r="H14" t="s">
+        <v>147</v>
+      </c>
+      <c r="J14" t="s">
         <v>144</v>
       </c>
-      <c r="H14" t="s">
-        <v>149</v>
-      </c>
-      <c r="J14" t="s">
-        <v>145</v>
-      </c>
       <c r="K14" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -2110,19 +2098,19 @@
         <v>133</v>
       </c>
       <c r="H15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -2157,28 +2145,28 @@
         <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F16" t="s">
         <v>125</v>
       </c>
       <c r="G16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H16" t="s">
+        <v>147</v>
+      </c>
+      <c r="J16" t="s">
         <v>149</v>
       </c>
-      <c r="J16" t="s">
-        <v>151</v>
-      </c>
       <c r="K16" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M16" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -2219,25 +2207,25 @@
         <v>125</v>
       </c>
       <c r="G17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M17" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -2278,22 +2266,22 @@
         <v>125</v>
       </c>
       <c r="G18" t="s">
+        <v>153</v>
+      </c>
+      <c r="H18" t="s">
+        <v>154</v>
+      </c>
+      <c r="I18" t="s">
         <v>155</v>
       </c>
-      <c r="H18" t="s">
-        <v>156</v>
-      </c>
-      <c r="I18" t="s">
-        <v>157</v>
-      </c>
       <c r="K18" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M18" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="N18">
         <v>0</v>
@@ -2334,22 +2322,22 @@
         <v>125</v>
       </c>
       <c r="G19" t="s">
+        <v>156</v>
+      </c>
+      <c r="H19" t="s">
+        <v>157</v>
+      </c>
+      <c r="J19" t="s">
         <v>158</v>
       </c>
-      <c r="H19" t="s">
-        <v>159</v>
-      </c>
-      <c r="J19" t="s">
-        <v>160</v>
-      </c>
       <c r="K19" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L19" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L19" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M19" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -2372,7 +2360,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B20" t="s">
         <v>66</v>
@@ -2390,19 +2378,19 @@
         <v>125</v>
       </c>
       <c r="G20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -2425,7 +2413,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B21" t="s">
         <v>66</v>
@@ -2434,7 +2422,7 @@
         <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E21" t="s">
         <v>76</v>
@@ -2443,22 +2431,22 @@
         <v>125</v>
       </c>
       <c r="G21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K21" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L21" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M21" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N21">
         <v>0</v>
@@ -2499,19 +2487,19 @@
         <v>125</v>
       </c>
       <c r="G22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J22" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="K22" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L22" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M22" s="2" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -2543,7 +2531,7 @@
         <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E23" t="s">
         <v>79</v>
@@ -2552,22 +2540,22 @@
         <v>125</v>
       </c>
       <c r="G23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K23" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L23" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M23" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -2608,25 +2596,25 @@
         <v>125</v>
       </c>
       <c r="G24" t="s">
+        <v>167</v>
+      </c>
+      <c r="H24" t="s">
+        <v>164</v>
+      </c>
+      <c r="I24" t="s">
+        <v>168</v>
+      </c>
+      <c r="J24" t="s">
         <v>169</v>
       </c>
-      <c r="H24" t="s">
-        <v>166</v>
-      </c>
-      <c r="I24" t="s">
-        <v>170</v>
-      </c>
-      <c r="J24" t="s">
-        <v>171</v>
-      </c>
       <c r="K24" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L24" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M24" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -2667,22 +2655,22 @@
         <v>125</v>
       </c>
       <c r="G25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H25" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K25" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L25" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M25" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -2723,16 +2711,16 @@
         <v>125</v>
       </c>
       <c r="G26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -2773,16 +2761,16 @@
         <v>125</v>
       </c>
       <c r="G27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -2823,16 +2811,16 @@
         <v>125</v>
       </c>
       <c r="G28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -2873,16 +2861,16 @@
         <v>125</v>
       </c>
       <c r="G29" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -2905,7 +2893,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B30" t="s">
         <v>109</v>
@@ -2923,16 +2911,16 @@
         <v>125</v>
       </c>
       <c r="G30" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N30">
         <v>0</v>
@@ -2973,16 +2961,16 @@
         <v>125</v>
       </c>
       <c r="G31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N31">
         <v>0</v>

</xml_diff>

<commit_message>
small shou-hua bug fix sign)extend -> sign_extend
</commit_message>
<xml_diff>
--- a/doc/pr2_design/instruction.xlsx
+++ b/doc/pr2_design/instruction.xlsx
@@ -418,23 +418,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>if (R[x]=0) then PC←PC+sign)extend(immediate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BTEQZ immediate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>if (T=0) then PC←PC+sign)extend(immediate)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BNEZ rx immediate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>if (R[x]!=0) then PC←PC+sign)extend(immediate)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -932,6 +920,18 @@
   </si>
   <si>
     <t>A←ry, B←zero_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (T=0) then PC←PC+sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (R[x]=0) then PC←PC+sign_extend(immediate)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (R[x]!=0) then PC←PC+sign_extend(immediate)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1301,10 +1301,10 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1335,72 +1335,72 @@
         <v>30</v>
       </c>
       <c r="F1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" t="s">
         <v>120</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>121</v>
       </c>
-      <c r="H1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" t="s">
-        <v>124</v>
-      </c>
       <c r="K1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="N1" t="s">
+        <v>184</v>
+      </c>
+      <c r="O1" t="s">
+        <v>180</v>
+      </c>
+      <c r="P1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q1" t="s">
         <v>182</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="N1" t="s">
-        <v>187</v>
-      </c>
-      <c r="O1" t="s">
-        <v>183</v>
-      </c>
-      <c r="P1" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>185</v>
-      </c>
       <c r="R1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="S1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1438,22 +1438,22 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -1491,22 +1491,22 @@
         <v>34</v>
       </c>
       <c r="F4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" t="s">
         <v>126</v>
       </c>
-      <c r="G4" t="s">
-        <v>129</v>
-      </c>
       <c r="J4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>193</v>
-      </c>
       <c r="M4" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1544,22 +1544,22 @@
         <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1597,22 +1597,22 @@
         <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1650,25 +1650,25 @@
         <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -1706,25 +1706,25 @@
         <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G8" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" t="s">
         <v>133</v>
       </c>
-      <c r="H8" t="s">
-        <v>136</v>
-      </c>
       <c r="J8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -1762,25 +1762,25 @@
         <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="J9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
@@ -1818,22 +1818,22 @@
         <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1871,22 +1871,22 @@
         <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -1924,25 +1924,25 @@
         <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G12" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1980,25 +1980,25 @@
         <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G13" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -2036,25 +2036,25 @@
         <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K14" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="M14" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -2092,25 +2092,25 @@
         <v>55</v>
       </c>
       <c r="F15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J15" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -2145,28 +2145,28 @@
         <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G16" t="s">
+        <v>143</v>
+      </c>
+      <c r="H16" t="s">
+        <v>144</v>
+      </c>
+      <c r="J16" t="s">
         <v>146</v>
       </c>
-      <c r="H16" t="s">
-        <v>147</v>
-      </c>
-      <c r="J16" t="s">
-        <v>149</v>
-      </c>
       <c r="K16" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -2204,28 +2204,28 @@
         <v>71</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G17" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H17" t="s">
+        <v>144</v>
+      </c>
+      <c r="I17" t="s">
         <v>147</v>
       </c>
-      <c r="I17" t="s">
-        <v>150</v>
-      </c>
       <c r="J17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -2263,25 +2263,25 @@
         <v>84</v>
       </c>
       <c r="F18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="N18">
         <v>0</v>
@@ -2319,25 +2319,25 @@
         <v>73</v>
       </c>
       <c r="F19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G19" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -2360,7 +2360,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B20" t="s">
         <v>66</v>
@@ -2375,22 +2375,22 @@
         <v>75</v>
       </c>
       <c r="F20" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G20" t="s">
+        <v>153</v>
+      </c>
+      <c r="H20" t="s">
         <v>156</v>
       </c>
-      <c r="H20" t="s">
-        <v>159</v>
-      </c>
       <c r="K20" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -2413,7 +2413,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B21" t="s">
         <v>66</v>
@@ -2422,31 +2422,31 @@
         <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E21" t="s">
         <v>76</v>
       </c>
       <c r="F21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H21" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="J21" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="N21">
         <v>0</v>
@@ -2484,22 +2484,22 @@
         <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G22" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J22" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -2531,31 +2531,31 @@
         <v>88</v>
       </c>
       <c r="D23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E23" t="s">
         <v>79</v>
       </c>
       <c r="F23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G23" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H23" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J23" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -2593,28 +2593,28 @@
         <v>101</v>
       </c>
       <c r="F24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G24" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H24" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I24" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -2652,25 +2652,25 @@
         <v>82</v>
       </c>
       <c r="F25" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G25" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H25" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="I25" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -2705,22 +2705,22 @@
         <v>100</v>
       </c>
       <c r="E26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -2752,25 +2752,25 @@
         <v>93</v>
       </c>
       <c r="D27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E27" t="s">
-        <v>105</v>
+        <v>220</v>
       </c>
       <c r="F27" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G27" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -2805,22 +2805,22 @@
         <v>102</v>
       </c>
       <c r="E28" t="s">
-        <v>103</v>
+        <v>221</v>
       </c>
       <c r="F28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -2852,25 +2852,25 @@
         <v>97</v>
       </c>
       <c r="D29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E29" t="s">
-        <v>107</v>
+        <v>222</v>
       </c>
       <c r="F29" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G29" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -2893,34 +2893,34 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" t="s">
         <v>111</v>
       </c>
-      <c r="D30" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" t="s">
-        <v>114</v>
-      </c>
       <c r="F30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G30" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N30">
         <v>0</v>
@@ -2943,34 +2943,34 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D31" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E31" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G31" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N31">
         <v>0</v>

</xml_diff>

<commit_message>
fixed MTSP, add mux_clk
</commit_message>
<xml_diff>
--- a/doc/pr2_design/instruction.xlsx
+++ b/doc/pr2_design/instruction.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="10470" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="223">
   <si>
     <t>指令</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1301,10 +1301,10 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1630,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.15">

</xml_diff>